<commit_message>
cambios en arca 2 28.07.2025
</commit_message>
<xml_diff>
--- a/Capitulo999_INSTITUTO/Taller1_2025/AlumnosTaller1_2025.xlsx
+++ b/Capitulo999_INSTITUTO/Taller1_2025/AlumnosTaller1_2025.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6317A29C-C247-45AB-BBB8-60F7E6A4E177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$C$2:$G$68</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$C$2:$I$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Hoja2!$B$3:$G$3</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="65">
   <si>
     <t>Control</t>
   </si>
@@ -121,9 +123,6 @@
     <t>ROBERT , MARIANO</t>
   </si>
   <si>
-    <t>CHAILE , TAMARA FLORENCIA</t>
-  </si>
-  <si>
     <t>APROBADO</t>
   </si>
   <si>
@@ -187,13 +186,46 @@
     <t>chico de rulitos que nunca presentó nada</t>
   </si>
   <si>
-    <t>Aprobado</t>
+    <t>UNIDAD 1</t>
+  </si>
+  <si>
+    <t>UNIDAD 2</t>
+  </si>
+  <si>
+    <t>UNIDAD 3</t>
+  </si>
+  <si>
+    <t>UNIDAD 4</t>
+  </si>
+  <si>
+    <t>APELLIDO Y NOMBRE</t>
+  </si>
+  <si>
+    <t>Registrado</t>
+  </si>
+  <si>
+    <t>TALLER DE DISEÑO DE SOFTWARE I - 2025 - ING. DANIEL MALDONADO</t>
+  </si>
+  <si>
+    <t>Aprobado Unidad 2</t>
+  </si>
+  <si>
+    <t>ASISTENCIA</t>
+  </si>
+  <si>
+    <t>Situacion</t>
+  </si>
+  <si>
+    <t>Estuvo presente</t>
+  </si>
+  <si>
+    <t>SIN EVALUAC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0.00"/>
   </numFmts>
@@ -214,7 +246,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -239,8 +271,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA3DBFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF29B95C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF227ACB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -248,11 +316,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -261,6 +344,18 @@
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,27 +635,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H84"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:I84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C70" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C63" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B73" sqref="B73"/>
+      <selection pane="bottomRight" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="2.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" customWidth="1"/>
-    <col min="7" max="7" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
@@ -576,83 +673,134 @@
       <c r="G2" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>26</v>
       </c>
@@ -663,35 +811,53 @@
         <v>1</v>
       </c>
       <c r="G18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="I18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>25</v>
       </c>
@@ -707,8 +873,11 @@
       <c r="G24" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>11</v>
       </c>
@@ -724,8 +893,11 @@
       <c r="G25" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>12</v>
       </c>
@@ -738,8 +910,11 @@
       <c r="F26">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>23</v>
       </c>
@@ -752,8 +927,11 @@
       <c r="F27">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>13</v>
       </c>
@@ -766,8 +944,11 @@
       <c r="F28">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>18</v>
       </c>
@@ -783,8 +964,11 @@
       <c r="G29" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>15</v>
       </c>
@@ -800,8 +984,11 @@
       <c r="G30" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>16</v>
       </c>
@@ -817,10 +1004,13 @@
       <c r="G31" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I31" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="D32" s="2">
         <v>45793</v>
@@ -834,8 +1024,11 @@
       <c r="G32" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>14</v>
       </c>
@@ -848,8 +1041,11 @@
       <c r="F33">
         <v>7</v>
       </c>
-    </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I33" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>28</v>
       </c>
@@ -865,8 +1061,11 @@
       <c r="G34" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>12</v>
       </c>
@@ -874,13 +1073,16 @@
         <v>45800</v>
       </c>
       <c r="G35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H35" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="I35" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>25</v>
       </c>
@@ -888,13 +1090,16 @@
         <v>45800</v>
       </c>
       <c r="G36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H36" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="3:8" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="I36" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>14</v>
       </c>
@@ -902,13 +1107,16 @@
         <v>45800</v>
       </c>
       <c r="G37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H37" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="38" spans="3:8" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="I37" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>15</v>
       </c>
@@ -916,13 +1124,16 @@
         <v>45800</v>
       </c>
       <c r="G38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="39" spans="3:8" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="I38" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
         <v>13</v>
       </c>
@@ -930,13 +1141,16 @@
         <v>45800</v>
       </c>
       <c r="G39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H39" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="40" spans="3:8" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="I39" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>13</v>
       </c>
@@ -950,15 +1164,18 @@
         <v>15</v>
       </c>
       <c r="G40" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H40" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="41" spans="3:8" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="I40" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="D41" s="2">
         <v>45807</v>
@@ -970,10 +1187,13 @@
         <v>30</v>
       </c>
       <c r="G41" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="42" spans="3:8" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="I41" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
         <v>11</v>
       </c>
@@ -987,10 +1207,13 @@
         <v>12</v>
       </c>
       <c r="G42" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="43" spans="3:8" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="I42" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
         <v>28</v>
       </c>
@@ -1004,10 +1227,13 @@
         <v>8</v>
       </c>
       <c r="G43" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="44" spans="3:8" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="I43" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
         <v>23</v>
       </c>
@@ -1020,8 +1246,11 @@
       <c r="F44">
         <v>12</v>
       </c>
-    </row>
-    <row r="45" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I44" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
         <v>27</v>
       </c>
@@ -1034,8 +1263,11 @@
       <c r="F45">
         <v>8</v>
       </c>
-    </row>
-    <row r="46" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I45" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="46" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
         <v>14</v>
       </c>
@@ -1048,8 +1280,11 @@
       <c r="F46">
         <v>18</v>
       </c>
-    </row>
-    <row r="47" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I46" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
         <v>25</v>
       </c>
@@ -1062,8 +1297,11 @@
       <c r="F47">
         <v>15</v>
       </c>
-    </row>
-    <row r="48" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I47" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
         <v>15</v>
       </c>
@@ -1077,15 +1315,18 @@
         <v>18</v>
       </c>
       <c r="G48" t="s">
+        <v>38</v>
+      </c>
+      <c r="I48" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>46</v>
+      </c>
+      <c r="C49" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>47</v>
-      </c>
-      <c r="C49" t="s">
-        <v>40</v>
       </c>
       <c r="D49" s="2">
         <v>45814</v>
@@ -1094,12 +1335,15 @@
         <v>1</v>
       </c>
       <c r="G49" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="I49" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>16</v>
@@ -1110,12 +1354,15 @@
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
       <c r="G50" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="I50" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C51" t="s">
         <v>11</v>
@@ -1124,12 +1371,15 @@
         <v>45814</v>
       </c>
       <c r="G51" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="I51" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C52" t="s">
         <v>31</v>
@@ -1138,15 +1388,18 @@
         <v>45814</v>
       </c>
       <c r="G52" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="I52" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C53" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D53" s="2">
         <v>45814</v>
@@ -1158,12 +1411,15 @@
         <v>11</v>
       </c>
       <c r="G53" t="s">
+        <v>45</v>
+      </c>
+      <c r="I53" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>47</v>
       </c>
       <c r="C54" t="s">
         <v>27</v>
@@ -1177,10 +1433,13 @@
       <c r="F54">
         <v>25</v>
       </c>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I54" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C55" t="s">
         <v>30</v>
@@ -1192,12 +1451,15 @@
         <v>1</v>
       </c>
       <c r="G55" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="I55" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C56" t="s">
         <v>24</v>
@@ -1211,13 +1473,16 @@
       <c r="F56">
         <v>3</v>
       </c>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I56" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
+        <v>46</v>
+      </c>
+      <c r="C57" t="s">
         <v>47</v>
-      </c>
-      <c r="C57" t="s">
-        <v>48</v>
       </c>
       <c r="D57" s="2">
         <v>45814</v>
@@ -1226,7 +1491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
         <v>12</v>
       </c>
@@ -1234,10 +1499,16 @@
         <v>45819</v>
       </c>
       <c r="G58" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="H58" t="s">
+        <v>32</v>
+      </c>
+      <c r="I58" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
         <v>23</v>
       </c>
@@ -1245,10 +1516,16 @@
         <v>45819</v>
       </c>
       <c r="G59" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="H59" t="s">
+        <v>32</v>
+      </c>
+      <c r="I59" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
         <v>25</v>
       </c>
@@ -1256,10 +1533,16 @@
         <v>45819</v>
       </c>
       <c r="G60" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="H60" t="s">
+        <v>32</v>
+      </c>
+      <c r="I60" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
         <v>13</v>
       </c>
@@ -1267,10 +1550,16 @@
         <v>45819</v>
       </c>
       <c r="G61" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="H61" t="s">
+        <v>32</v>
+      </c>
+      <c r="I61" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
         <v>14</v>
       </c>
@@ -1278,10 +1567,16 @@
         <v>45819</v>
       </c>
       <c r="G62" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="H62" t="s">
+        <v>32</v>
+      </c>
+      <c r="I62" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
         <v>18</v>
       </c>
@@ -1289,10 +1584,16 @@
         <v>45821</v>
       </c>
       <c r="G63" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="H63" t="s">
+        <v>32</v>
+      </c>
+      <c r="I63" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
         <v>22</v>
       </c>
@@ -1300,10 +1601,16 @@
         <v>45821</v>
       </c>
       <c r="G64" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="65" spans="3:7" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="H64" t="s">
+        <v>32</v>
+      </c>
+      <c r="I64" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="65" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
         <v>26</v>
       </c>
@@ -1311,10 +1618,16 @@
         <v>45821</v>
       </c>
       <c r="G65" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="66" spans="3:7" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="H65" t="s">
+        <v>32</v>
+      </c>
+      <c r="I65" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="66" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C66" t="s">
         <v>27</v>
       </c>
@@ -1322,10 +1635,16 @@
         <v>45821</v>
       </c>
       <c r="G66" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="67" spans="3:7" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="H66" t="s">
+        <v>32</v>
+      </c>
+      <c r="I66" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="67" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
         <v>11</v>
       </c>
@@ -1333,10 +1652,16 @@
         <v>45821</v>
       </c>
       <c r="G67" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="68" spans="3:7" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="H67" t="s">
+        <v>32</v>
+      </c>
+      <c r="I67" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="68" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
         <v>15</v>
       </c>
@@ -1344,18 +1669,27 @@
         <v>45821</v>
       </c>
       <c r="G68" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="69" spans="3:7" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="H68" t="s">
+        <v>32</v>
+      </c>
+      <c r="I68" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="69" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C69" t="s">
         <v>11</v>
       </c>
       <c r="D69" s="2">
         <v>45840</v>
       </c>
-    </row>
-    <row r="70" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="I69" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="70" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C70" t="s">
         <v>13</v>
       </c>
@@ -1363,10 +1697,16 @@
         <v>45840</v>
       </c>
       <c r="G70" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="71" spans="3:7" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="H70" t="s">
+        <v>32</v>
+      </c>
+      <c r="I70" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="71" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
         <v>14</v>
       </c>
@@ -1374,10 +1714,16 @@
         <v>45840</v>
       </c>
       <c r="G71" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="72" spans="3:7" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="H71" t="s">
+        <v>32</v>
+      </c>
+      <c r="I71" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="72" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
         <v>15</v>
       </c>
@@ -1385,10 +1731,16 @@
         <v>45840</v>
       </c>
       <c r="G72" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="73" spans="3:7" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="H72" t="s">
+        <v>32</v>
+      </c>
+      <c r="I72" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="73" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C73" t="s">
         <v>16</v>
       </c>
@@ -1396,28 +1748,46 @@
         <v>45840</v>
       </c>
       <c r="G73" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="74" spans="3:7" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="H73" t="s">
+        <v>32</v>
+      </c>
+      <c r="I73" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="74" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C74" t="s">
         <v>18</v>
       </c>
       <c r="D74" s="2">
         <v>45840</v>
       </c>
-    </row>
-    <row r="75" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G74" t="s">
+        <v>63</v>
+      </c>
+      <c r="I74" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="75" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C75" t="s">
         <v>12</v>
       </c>
       <c r="D75" s="2">
         <v>45840</v>
       </c>
-    </row>
-    <row r="76" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G75" t="s">
+        <v>63</v>
+      </c>
+      <c r="I75" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="76" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C76" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D76" s="7">
         <v>45840</v>
@@ -1425,10 +1795,13 @@
       <c r="E76" s="6"/>
       <c r="F76" s="6"/>
       <c r="G76" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="77" spans="3:7" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="I76" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="77" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C77" s="6" t="s">
         <v>20</v>
       </c>
@@ -1438,34 +1811,55 @@
       <c r="E77" s="6"/>
       <c r="F77" s="6"/>
       <c r="G77" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="78" spans="3:7" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="I77" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="78" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C78" t="s">
         <v>23</v>
       </c>
       <c r="D78" s="2">
         <v>45840</v>
       </c>
-    </row>
-    <row r="79" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G78" t="s">
+        <v>63</v>
+      </c>
+      <c r="I78" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="79" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C79" t="s">
         <v>22</v>
       </c>
       <c r="D79" s="2">
         <v>45840</v>
       </c>
-    </row>
-    <row r="80" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G79" t="s">
+        <v>63</v>
+      </c>
+      <c r="I79" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="80" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C80" t="s">
         <v>27</v>
       </c>
       <c r="D80" s="2">
         <v>45840</v>
       </c>
-    </row>
-    <row r="81" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G80" t="s">
+        <v>63</v>
+      </c>
+      <c r="I80" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="81" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C81" s="6" t="s">
         <v>24</v>
       </c>
@@ -1475,10 +1869,13 @@
       <c r="E81" s="6"/>
       <c r="F81" s="6"/>
       <c r="G81" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="82" spans="3:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="I81" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="82" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C82" t="s">
         <v>25</v>
       </c>
@@ -1486,10 +1883,16 @@
         <v>45840</v>
       </c>
       <c r="G82" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="83" spans="3:7" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="H82" t="s">
+        <v>32</v>
+      </c>
+      <c r="I82" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="83" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C83" s="6" t="s">
         <v>31</v>
       </c>
@@ -1499,49 +1902,455 @@
       <c r="E83" s="6"/>
       <c r="F83" s="6"/>
       <c r="G83" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="84" spans="3:7" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="I83" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="84" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C84" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D84" s="2">
         <v>45840</v>
       </c>
+      <c r="G84" t="s">
+        <v>63</v>
+      </c>
+      <c r="I84" t="s">
+        <v>58</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="C2:G68"/>
+  <autoFilter ref="C2:I2" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D5:H5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B2:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="13.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="6" max="7" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D5" s="3">
-        <v>1200000</v>
-      </c>
-      <c r="F5">
-        <v>100</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="13">
+        <v>2</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="16">
+        <v>1</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="16">
+        <v>1</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="16">
+        <v>1</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="16">
+        <v>1</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="16">
+        <v>1</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="16">
+        <v>2</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="16">
+        <v>1</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="16">
+        <v>1</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="16">
+        <v>1</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="16">
+        <v>1</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="16">
+        <v>1</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="16">
+        <v>1</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="16">
+        <v>2</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="16">
+        <v>2</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="16">
+        <v>1</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="16">
+        <v>1</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="16">
+        <v>2</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="13">
+        <v>1</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="16">
+        <v>1</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="16">
+        <v>2</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="16">
+        <v>2</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="16">
+        <v>1</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="16">
+        <v>1</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
   </sheetData>
+  <autoFilter ref="B3:G3" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:G27">
+    <sortCondition ref="C4:C27"/>
+  </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="B2:G2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
cambios en casa 18.08.2025
</commit_message>
<xml_diff>
--- a/Capitulo999_INSTITUTO/Taller1_2025/AlumnosTaller1_2025.xlsx
+++ b/Capitulo999_INSTITUTO/Taller1_2025/AlumnosTaller1_2025.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6317A29C-C247-45AB-BBB8-60F7E6A4E177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$C$2:$I$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$C$2:$J$85</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Hoja2!$B$3:$G$3</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="70">
   <si>
     <t>Control</t>
   </si>
@@ -220,16 +219,31 @@
   </si>
   <si>
     <t>SIN EVALUAC</t>
+  </si>
+  <si>
+    <t>Cuatrimestre</t>
+  </si>
+  <si>
+    <t>primero</t>
+  </si>
+  <si>
+    <t>segundo</t>
+  </si>
+  <si>
+    <t>32, 34</t>
+  </si>
+  <si>
+    <t>presentó la guía 1 a medias. No puede explicar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,6 +255,19 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -335,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -346,9 +373,6 @@
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -356,6 +380,11 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -635,14 +664,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:I84"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
+  <dimension ref="B2:J1048576"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C63" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C88" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D35" sqref="D35"/>
+      <selection pane="bottomRight" activeCell="G92" sqref="G92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,9 +685,10 @@
     <col min="7" max="7" width="46.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
@@ -679,128 +710,176 @@
       <c r="I2" s="9" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>11</v>
       </c>
       <c r="I3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>12</v>
       </c>
       <c r="I4" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>13</v>
       </c>
       <c r="I5" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>14</v>
       </c>
       <c r="I6" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>15</v>
       </c>
       <c r="I7" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>16</v>
       </c>
       <c r="I8" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>17</v>
       </c>
       <c r="I9" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>18</v>
       </c>
       <c r="I10" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>19</v>
       </c>
       <c r="I11" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>20</v>
       </c>
       <c r="I12" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>21</v>
       </c>
       <c r="I13" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>22</v>
       </c>
       <c r="I14" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>23</v>
       </c>
       <c r="I15" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>24</v>
       </c>
       <c r="I16" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>25</v>
       </c>
       <c r="I17" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>26</v>
       </c>
@@ -816,48 +895,66 @@
       <c r="I18" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>27</v>
       </c>
       <c r="I19" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>28</v>
       </c>
       <c r="I20" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>29</v>
       </c>
       <c r="I21" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>30</v>
       </c>
       <c r="I22" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>31</v>
       </c>
       <c r="I23" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>25</v>
       </c>
@@ -876,8 +973,11 @@
       <c r="I24" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>11</v>
       </c>
@@ -896,8 +996,11 @@
       <c r="I25" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>12</v>
       </c>
@@ -913,8 +1016,11 @@
       <c r="I26" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>23</v>
       </c>
@@ -930,8 +1036,11 @@
       <c r="I27" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>13</v>
       </c>
@@ -947,8 +1056,11 @@
       <c r="I28" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>18</v>
       </c>
@@ -967,8 +1079,11 @@
       <c r="I29" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="30" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>15</v>
       </c>
@@ -987,8 +1102,11 @@
       <c r="I30" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>16</v>
       </c>
@@ -1007,8 +1125,11 @@
       <c r="I31" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="32" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J31" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>22</v>
       </c>
@@ -1027,8 +1148,11 @@
       <c r="I32" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J32" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>14</v>
       </c>
@@ -1044,8 +1168,11 @@
       <c r="I33" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J33" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>28</v>
       </c>
@@ -1064,8 +1191,11 @@
       <c r="I34" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>12</v>
       </c>
@@ -1081,8 +1211,11 @@
       <c r="I35" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>25</v>
       </c>
@@ -1098,8 +1231,11 @@
       <c r="I36" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="37" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J36" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>14</v>
       </c>
@@ -1115,8 +1251,11 @@
       <c r="I37" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="38" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J37" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>15</v>
       </c>
@@ -1132,8 +1271,11 @@
       <c r="I38" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="39" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J38" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
         <v>13</v>
       </c>
@@ -1149,8 +1291,11 @@
       <c r="I39" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="40" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J39" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>13</v>
       </c>
@@ -1172,8 +1317,11 @@
       <c r="I40" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="41" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J40" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
         <v>22</v>
       </c>
@@ -1192,8 +1340,11 @@
       <c r="I41" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="42" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J41" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
         <v>11</v>
       </c>
@@ -1212,8 +1363,11 @@
       <c r="I42" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="43" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J42" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
         <v>28</v>
       </c>
@@ -1232,8 +1386,11 @@
       <c r="I43" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="44" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J43" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
         <v>23</v>
       </c>
@@ -1249,8 +1406,11 @@
       <c r="I44" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="45" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J44" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
         <v>27</v>
       </c>
@@ -1266,8 +1426,11 @@
       <c r="I45" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="46" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J45" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="46" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
         <v>14</v>
       </c>
@@ -1283,8 +1446,11 @@
       <c r="I46" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="47" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J46" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="47" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
         <v>25</v>
       </c>
@@ -1300,8 +1466,11 @@
       <c r="I47" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="48" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J47" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="48" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
         <v>15</v>
       </c>
@@ -1320,8 +1489,11 @@
       <c r="I48" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J48" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>46</v>
       </c>
@@ -1340,8 +1512,11 @@
       <c r="I49" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J49" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>46</v>
       </c>
@@ -1359,8 +1534,11 @@
       <c r="I50" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J50" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>46</v>
       </c>
@@ -1376,8 +1554,11 @@
       <c r="I51" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J51" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>46</v>
       </c>
@@ -1393,8 +1574,11 @@
       <c r="I52" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J52" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>46</v>
       </c>
@@ -1416,8 +1600,11 @@
       <c r="I53" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J53" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>46</v>
       </c>
@@ -1436,8 +1623,11 @@
       <c r="I54" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J54" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>46</v>
       </c>
@@ -1456,8 +1646,11 @@
       <c r="I55" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J55" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>46</v>
       </c>
@@ -1476,8 +1669,11 @@
       <c r="I56" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J56" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>46</v>
       </c>
@@ -1490,8 +1686,11 @@
       <c r="E57">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J57" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
         <v>12</v>
       </c>
@@ -1507,8 +1706,11 @@
       <c r="I58" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J58" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
         <v>23</v>
       </c>
@@ -1524,8 +1726,11 @@
       <c r="I59" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J59" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
         <v>25</v>
       </c>
@@ -1541,8 +1746,11 @@
       <c r="I60" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J60" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="61" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
         <v>13</v>
       </c>
@@ -1558,8 +1766,11 @@
       <c r="I61" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J61" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="62" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
         <v>14</v>
       </c>
@@ -1575,8 +1786,11 @@
       <c r="I62" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J62" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="63" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
         <v>18</v>
       </c>
@@ -1592,8 +1806,11 @@
       <c r="I63" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J63" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="64" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
         <v>22</v>
       </c>
@@ -1609,8 +1826,11 @@
       <c r="I64" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="65" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J64" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="65" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
         <v>26</v>
       </c>
@@ -1626,8 +1846,11 @@
       <c r="I65" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="66" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J65" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="66" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C66" t="s">
         <v>27</v>
       </c>
@@ -1643,8 +1866,11 @@
       <c r="I66" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="67" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J66" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
         <v>11</v>
       </c>
@@ -1660,8 +1886,11 @@
       <c r="I67" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="68" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J67" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
         <v>15</v>
       </c>
@@ -1677,8 +1906,11 @@
       <c r="I68" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="69" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J68" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C69" t="s">
         <v>11</v>
       </c>
@@ -1688,8 +1920,11 @@
       <c r="I69" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="70" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J69" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="70" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C70" t="s">
         <v>13</v>
       </c>
@@ -1705,8 +1940,11 @@
       <c r="I70" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="71" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J70" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="71" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
         <v>14</v>
       </c>
@@ -1722,8 +1960,11 @@
       <c r="I71" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="72" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J71" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="72" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
         <v>15</v>
       </c>
@@ -1739,8 +1980,11 @@
       <c r="I72" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="73" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J72" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="73" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C73" t="s">
         <v>16</v>
       </c>
@@ -1756,8 +2000,11 @@
       <c r="I73" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="74" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J73" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="74" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C74" t="s">
         <v>18</v>
       </c>
@@ -1770,8 +2017,11 @@
       <c r="I74" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="75" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J74" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="75" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C75" t="s">
         <v>12</v>
       </c>
@@ -1784,8 +2034,11 @@
       <c r="I75" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="76" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J75" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="76" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C76" s="6" t="s">
         <v>39</v>
       </c>
@@ -1800,8 +2053,11 @@
       <c r="I76" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="77" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J76" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="77" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C77" s="6" t="s">
         <v>20</v>
       </c>
@@ -1816,8 +2072,11 @@
       <c r="I77" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="78" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J77" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="78" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C78" t="s">
         <v>23</v>
       </c>
@@ -1830,8 +2089,11 @@
       <c r="I78" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="79" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J78" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="79" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C79" t="s">
         <v>22</v>
       </c>
@@ -1844,8 +2106,11 @@
       <c r="I79" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="80" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J79" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="80" spans="3:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C80" t="s">
         <v>27</v>
       </c>
@@ -1858,8 +2123,11 @@
       <c r="I80" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="81" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J80" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="81" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C81" s="6" t="s">
         <v>24</v>
       </c>
@@ -1874,8 +2142,11 @@
       <c r="I81" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="82" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J81" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="82" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C82" t="s">
         <v>25</v>
       </c>
@@ -1891,8 +2162,11 @@
       <c r="I82" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="83" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J82" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="83" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C83" s="6" t="s">
         <v>31</v>
       </c>
@@ -1907,8 +2181,11 @@
       <c r="I83" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="84" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J83" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="84" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="C84" t="s">
         <v>44</v>
       </c>
@@ -1921,19 +2198,237 @@
       <c r="I84" t="s">
         <v>58</v>
       </c>
+      <c r="J84" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="85" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C85" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D85" s="2">
+        <v>45882</v>
+      </c>
+      <c r="E85">
+        <v>2</v>
+      </c>
+      <c r="G85" t="s">
+        <v>68</v>
+      </c>
+      <c r="J85" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="86" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C86" t="s">
+        <v>13</v>
+      </c>
+      <c r="D86" s="2">
+        <v>45882</v>
+      </c>
+      <c r="E86">
+        <v>2</v>
+      </c>
+      <c r="G86">
+        <v>46</v>
+      </c>
+      <c r="J86" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="87" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C87" t="s">
+        <v>39</v>
+      </c>
+      <c r="D87" s="2">
+        <v>45882</v>
+      </c>
+      <c r="E87">
+        <v>2</v>
+      </c>
+      <c r="G87" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="J87" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="88" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C88" t="s">
+        <v>14</v>
+      </c>
+      <c r="D88" s="2">
+        <v>45882</v>
+      </c>
+      <c r="E88">
+        <v>2</v>
+      </c>
+      <c r="G88">
+        <v>47</v>
+      </c>
+      <c r="J88" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="89" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C89" t="s">
+        <v>25</v>
+      </c>
+      <c r="D89" s="2">
+        <v>45882</v>
+      </c>
+      <c r="E89">
+        <v>2</v>
+      </c>
+      <c r="G89">
+        <v>37</v>
+      </c>
+      <c r="J89" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="90" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C90" t="s">
+        <v>15</v>
+      </c>
+      <c r="D90" s="2">
+        <v>45882</v>
+      </c>
+      <c r="E90">
+        <v>2</v>
+      </c>
+      <c r="G90">
+        <v>40</v>
+      </c>
+      <c r="J90" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="91" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B91" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C91" t="s">
+        <v>24</v>
+      </c>
+      <c r="D91" s="2">
+        <v>45882</v>
+      </c>
+    </row>
+    <row r="92" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C92" t="s">
+        <v>25</v>
+      </c>
+      <c r="D92" s="2">
+        <v>45882</v>
+      </c>
+    </row>
+    <row r="93" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C93" t="s">
+        <v>22</v>
+      </c>
+      <c r="D93" s="2">
+        <v>45882</v>
+      </c>
+    </row>
+    <row r="94" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B94" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C94" t="s">
+        <v>28</v>
+      </c>
+      <c r="D94" s="2">
+        <v>45882</v>
+      </c>
+    </row>
+    <row r="95" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B95" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C95" t="s">
+        <v>27</v>
+      </c>
+      <c r="D95" s="2">
+        <v>45882</v>
+      </c>
+    </row>
+    <row r="96" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B96" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C96" t="s">
+        <v>29</v>
+      </c>
+      <c r="D96" s="2">
+        <v>45882</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B97" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C97" t="s">
+        <v>44</v>
+      </c>
+      <c r="D97" s="2">
+        <v>45882</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B98" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C98" t="s">
+        <v>20</v>
+      </c>
+      <c r="D98" s="2">
+        <v>45882</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B99" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C99" t="s">
+        <v>39</v>
+      </c>
+      <c r="D99" s="2">
+        <v>45882</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B100" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C100" t="s">
+        <v>16</v>
+      </c>
+      <c r="D100" s="2">
+        <v>45882</v>
+      </c>
+    </row>
+    <row r="1048576" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D1048576" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="C2:I2" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="C2:J85">
+    <filterColumn colId="7">
+      <filters>
+        <filter val="segundo"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
@@ -1946,406 +2441,406 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="10" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="13">
+      <c r="B4" s="12">
         <v>2</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="16">
-        <v>1</v>
-      </c>
-      <c r="C5" s="14" t="s">
+      <c r="B5" s="15">
+        <v>1</v>
+      </c>
+      <c r="C5" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="16">
-        <v>1</v>
-      </c>
-      <c r="C6" s="14" t="s">
+      <c r="B6" s="15">
+        <v>1</v>
+      </c>
+      <c r="C6" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
+      <c r="D6" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="16">
-        <v>1</v>
-      </c>
-      <c r="C7" s="14" t="s">
+      <c r="B7" s="15">
+        <v>1</v>
+      </c>
+      <c r="C7" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
+      <c r="D7" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="16">
-        <v>1</v>
-      </c>
-      <c r="C8" s="14" t="s">
+      <c r="B8" s="15">
+        <v>1</v>
+      </c>
+      <c r="C8" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="16">
-        <v>1</v>
-      </c>
-      <c r="C9" s="13" t="s">
+      <c r="B9" s="15">
+        <v>1</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="D9" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="16">
+      <c r="B10" s="15">
         <v>2</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="16">
-        <v>1</v>
-      </c>
-      <c r="C11" s="14" t="s">
+      <c r="B11" s="15">
+        <v>1</v>
+      </c>
+      <c r="C11" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="D11" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="16">
-        <v>1</v>
-      </c>
-      <c r="C12" s="14" t="s">
+      <c r="B12" s="15">
+        <v>1</v>
+      </c>
+      <c r="C12" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="16">
-        <v>1</v>
-      </c>
-      <c r="C13" s="14" t="s">
+      <c r="B13" s="15">
+        <v>1</v>
+      </c>
+      <c r="C13" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="D13" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="16">
-        <v>1</v>
-      </c>
-      <c r="C14" s="14" t="s">
+      <c r="B14" s="15">
+        <v>1</v>
+      </c>
+      <c r="C14" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="D14" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="16">
-        <v>1</v>
-      </c>
-      <c r="C15" s="14" t="s">
+      <c r="B15" s="15">
+        <v>1</v>
+      </c>
+      <c r="C15" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="D15" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="16">
-        <v>1</v>
-      </c>
-      <c r="C16" s="14" t="s">
+      <c r="B16" s="15">
+        <v>1</v>
+      </c>
+      <c r="C16" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="D16" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="16">
+      <c r="B17" s="15">
         <v>2</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="16">
+      <c r="B18" s="15">
         <v>2</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="E18" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="16">
-        <v>1</v>
-      </c>
-      <c r="C19" s="14" t="s">
+      <c r="B19" s="15">
+        <v>1</v>
+      </c>
+      <c r="C19" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="D19" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="16">
-        <v>1</v>
-      </c>
-      <c r="C20" s="14" t="s">
+      <c r="B20" s="15">
+        <v>1</v>
+      </c>
+      <c r="C20" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="E20" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="16">
+      <c r="B21" s="15">
         <v>2</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="13">
-        <v>1</v>
-      </c>
-      <c r="C22" s="14" t="s">
+      <c r="B22" s="12">
+        <v>1</v>
+      </c>
+      <c r="C22" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="D22" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="16">
-        <v>1</v>
-      </c>
-      <c r="C23" s="14" t="s">
+      <c r="B23" s="15">
+        <v>1</v>
+      </c>
+      <c r="C23" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="D23" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="16">
+      <c r="B24" s="15">
         <v>2</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="E24" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="16">
+      <c r="B25" s="15">
         <v>2</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="D25" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E25" s="13" t="s">
+      <c r="E25" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="16">
-        <v>1</v>
-      </c>
-      <c r="C26" s="14" t="s">
+      <c r="B26" s="15">
+        <v>1</v>
+      </c>
+      <c r="C26" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="D26" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E26" s="13" t="s">
+      <c r="E26" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="16">
-        <v>1</v>
-      </c>
-      <c r="C27" s="14" t="s">
+      <c r="B27" s="15">
+        <v>1</v>
+      </c>
+      <c r="C27" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D27" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="D27" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
     </row>
   </sheetData>
-  <autoFilter ref="B3:G3" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:G27">
+  <autoFilter ref="B3:G3"/>
+  <sortState ref="B4:G27">
     <sortCondition ref="C4:C27"/>
   </sortState>
   <mergeCells count="1">

</xml_diff>

<commit_message>
cambios en arca 10.09.2025
</commit_message>
<xml_diff>
--- a/Capitulo999_INSTITUTO/Taller1_2025/AlumnosTaller1_2025.xlsx
+++ b/Capitulo999_INSTITUTO/Taller1_2025/AlumnosTaller1_2025.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541A16B3-AF7D-4FB2-8C44-F9BF257D69AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -275,7 +276,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0.00"/>
   </numFmts>
@@ -398,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -423,7 +424,6 @@
     <xf numFmtId="164" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -703,14 +703,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C127" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C112" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C137" sqref="C137"/>
+      <selection pane="bottomRight" activeCell="C113" sqref="C113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2722,7 +2722,7 @@
       </c>
     </row>
     <row r="129" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C129" s="22" t="s">
+      <c r="C129" t="s">
         <v>44</v>
       </c>
       <c r="D129" s="2">
@@ -2813,14 +2813,14 @@
       <c r="D1048576" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="C2:J133"/>
+  <autoFilter ref="C2:J133" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:G27"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -3234,8 +3234,8 @@
       <c r="G27" s="12"/>
     </row>
   </sheetData>
-  <autoFilter ref="B3:G3"/>
-  <sortState ref="B4:G27">
+  <autoFilter ref="B3:G3" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:G27">
     <sortCondition ref="C4:C27"/>
   </sortState>
   <mergeCells count="1">

</xml_diff>